<commit_message>
Telas alteradas e procedures adicionadas
</commit_message>
<xml_diff>
--- a/doc/Acompanhamento-e-avaliação-trabalho.xlsx
+++ b/doc/Acompanhamento-e-avaliação-trabalho.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="25200" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="25200" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Avaliação" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -273,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,14 +307,17 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,20 +613,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -727,8 +736,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D6" s="7">
-        <v>1</v>
+      <c r="D6" s="11">
+        <v>3</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -796,8 +805,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D9" s="13">
-        <v>3</v>
+      <c r="D9" s="11">
+        <v>1</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -914,7 +923,7 @@
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="3">
@@ -1183,10 +1192,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>25</v>
@@ -1254,20 +1263,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1815,10 +1824,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>25</v>

</xml_diff>